<commit_message>
added issue with Ryan's fix for extract.py
</commit_message>
<xml_diff>
--- a/Results/raresim_Beta Testing_Tracker.xlsx
+++ b/Results/raresim_Beta Testing_Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\raresim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02758A51-D905-44E1-8295-21E03E9EE98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC3432-9D17-4E33-B2A0-660BA859DBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="129">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1543,6 +1543,23 @@
   </si>
   <si>
     <t>When using RAREsim v2.1.1 to prune a starting haplotype file to 100% fun and syn and then to 80% fun and syn variants as detailed in 4 cells above, there is a discrepancy between the legend and pruned-variant legend files</t>
+  </si>
+  <si>
+    <t>Tried using Ryan's suggestion by first unzipping the .gz file e.g. 
+gzip -d &lt;filename&gt;.haps.gz
+and
+gunzip &lt;filename&gt;.haps.gz</t>
+  </si>
+  <si>
+    <t>Bug detected</t>
+  </si>
+  <si>
+    <t>-I would suggest fixing the extract.py code so that it can extract from a .haps.gz file or incorporate code in the extract.py function that first unzips the .haps.gz file so I don't have to do it outside of the framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-While this doesn't throw an error, it doesn't make sense in the framework of the code since the output of the sim.py function is a .gz file.
+-I would want to be able to smoothly transition from the sim.py code to the extract.py code without having to convert all of my hap files first
+</t>
   </si>
 </sst>
 </file>
@@ -2280,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2548,8 +2565,19 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+    <row r="32" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
@@ -2584,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -3094,22 +3122,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3336,21 +3354,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3375,9 +3400,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added comments for afs.py function
</commit_message>
<xml_diff>
--- a/Results/raresim_Beta Testing_Tracker.xlsx
+++ b/Results/raresim_Beta Testing_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC3432-9D17-4E33-B2A0-660BA859DBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE1063-75F8-4D65-848C-972B6558A899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="145">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1560,6 +1560,207 @@
     <t xml:space="preserve">-While this doesn't throw an error, it doesn't make sense in the framework of the code since the output of the sim.py function is a .gz file.
 -I would want to be able to smoothly transition from the sim.py code to the extract.py code without having to convert all of my hap files first
 </t>
+  </si>
+  <si>
+    <r>
+      <t>Function:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> afs.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameters (with default values, if any): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+    -h, --help               show this help message and exit
+    --pop POP             Population to use default values for
+    --mac MACS         csv file of MAC bins
+    --alpha ALPHA      Provided alpha value
+    --beta BETA           Provided beta value
+    -b B                        Provided b value
+    -o OUTPUT           Output file to be written</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Function:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nvariants.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate the total number of expected variants. This script simply outputs it's calculated value to the console, but if you want this to be written to a file you can add ` &gt; output.txt` to the end of the bash command to have it write the value to a file.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alternatively, you may provide your own omega and phi values if you have them.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameters (with default values, if any): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+  -h, --help                 show this help message and exit
+  --pop POP               Population to use default values for
+  --phi PHI                  Provided phi value
+  --omega ALPHA     Provided omega value
+  -N N                         Provided N value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Function:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> expected_variants.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate the number of expected variants per MAC bin based on the outputs from the afs and nvariant functions.
+Rows can be pruned allele by allele using probabilities given in the legend file.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameters (with default values, if any): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+  -h, --help               show this help message and exit
+  -N N                       Number of expected variants
+  --props PROPS     Provided mac bins with proportions
+  -o OUTPUT          Output file to be written</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate the frequencies with which you expect variants to appear in each MAC bin.
+Rows can be pruned allele by allele using probabilities given in the legend file. Alternatively, if you know your desired alpha, beta, and b parameters, you can also use those in place of the defaults for a given population.</t>
+    </r>
+  </si>
+  <si>
+    <t>example as given in the README
+--pop EAS 
+--mac testData/mac_bins.csv 
+-o /home/math/siglersa/sage_raresim/afs_test.txt</t>
+  </si>
+  <si>
+    <t>Maybe some more detail about what alpha, beta, and b parameters are</t>
+  </si>
+  <si>
+    <t>Would Include example output in README and some more description about the example</t>
+  </si>
+  <si>
+    <t>no comments in the actual afs.py file</t>
+  </si>
+  <si>
+    <t>Using NFE and my own input MAC bin csv file with 7 MAC bin sizes (1-1, 2-2, 3-5, 6-10, 11-20, 21-200, 201-400)
+--pop NFE 
+--mac /home/math/siglersa/sage_raresim/nfe_macs.csv 
+-o /home/math/siglersa/sage_raresim/afs_nfe_macs.txt</t>
+  </si>
+  <si>
+    <t>Again not sure if the probabilities should sum to 1 or not, this one sums to over 1</t>
+  </si>
+  <si>
+    <t>Not sure if the probabilities need to add up to 1 or not, this one sums to under 1</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2216,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2297,7 +2498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2612,7 +2813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -3087,47 +3288,632 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881D6BD8-94B7-4767-8C3D-2BA210E4CAAA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="124.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="39.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E12 E14:E16 E18" xr:uid="{CEB7DB4A-183A-425B-ACB3-1D397E993F4E}">
+      <formula1>"Reviewed, Not Reviewed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12 B14:B16 B18" xr:uid="{08BC3538-9A35-425B-8BD9-0DF6CB9B0EA7}">
+      <formula1>"Good, Needs Work"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B57A4DD-947A-4B6A-8176-CE02EE70EDC3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="119" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12 B14:B16 B18" xr:uid="{98E7A82C-232B-49F1-A0EB-ED5474918E49}">
+      <formula1>"Good, Needs Work"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E12 E14:E16 E18" xr:uid="{105F50F1-0ABC-4AFF-8181-CABFAA34C7E2}">
+      <formula1>"Reviewed, Not Reviewed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75856291-DF21-4AFA-91C0-857E3D86DCEF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="124.77734375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12 B14:B16 B18" xr:uid="{4A782F6C-C644-49F1-B64E-BEC17229CA57}">
+      <formula1>"Good, Needs Work"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E12 E14:E16 E18" xr:uid="{7C678A9A-1AA8-4E1C-B164-CFE3E12F68E1}">
+      <formula1>"Reviewed, Not Reviewed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3354,28 +4140,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3400,12 +4179,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added more notes to afs and nvariants functions
</commit_message>
<xml_diff>
--- a/Results/raresim_Beta Testing_Tracker.xlsx
+++ b/Results/raresim_Beta Testing_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE1063-75F8-4D65-848C-972B6558A899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5E9A83-ADB4-4BE4-9FEA-69D1FF757A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="149">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1761,6 +1761,51 @@
   </si>
   <si>
     <t>Not sure if the probabilities need to add up to 1 or not, this one sums to under 1</t>
+  </si>
+  <si>
+    <t>example as given in the README for alternate example
+ --alpha 1.5
+ --beta -.25
+ -b .25
+ --mac testData/mac_bins.csv
+ -o  /home/math/siglersa/sage_raresim/afs_param_test.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/afs.py", line 86, in &lt;module&gt;
+    afs()
+  File "/home/math/siglersa/raresim/afs.py", line 51, in afs
+    alpha = int(args.alpha)
+ValueError: invalid literal for int() with base 10: '1.5'</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given in the README
+-- pop AFR
+-N 15000</t>
+  </si>
+  <si>
+    <t>Tried as is and also using `&gt; output.txt` to save the output and both worked</t>
   </si>
 </sst>
 </file>
@@ -3290,15 +3335,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881D6BD8-94B7-4767-8C3D-2BA210E4CAAA}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="124.77734375" customWidth="1"/>
     <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="39.21875" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" customWidth="1"/>
     <col min="4" max="4" width="16.21875" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
@@ -3495,9 +3540,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3515,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B57A4DD-947A-4B6A-8176-CE02EE70EDC3}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3691,6 +3742,17 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3898,22 +3960,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4140,21 +4192,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4179,9 +4238,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added more notes to nvariants.py function
</commit_message>
<xml_diff>
--- a/Results/raresim_Beta Testing_Tracker.xlsx
+++ b/Results/raresim_Beta Testing_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5E9A83-ADB4-4BE4-9FEA-69D1FF757A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15F4D07-1E77-42EE-A22A-7614892E78AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="154">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1806,6 +1806,54 @@
   </si>
   <si>
     <t>Tried as is and also using `&gt; output.txt` to save the output and both worked</t>
+  </si>
+  <si>
+    <t>Alternative example as given in the README
+ --omega .15
+ --phi .65
+ -N 15000</t>
+  </si>
+  <si>
+    <t>-PROBLEM: on help menu, the --omega paramter has ALPHA listed next to it, but I'm assuming it should be OMEGA instead. Needs to be fixed.
+-Would also briefly describe what phi and omega are, and what N is (e.g. is N the number of individuals or the number of haplotypes?)</t>
+  </si>
+  <si>
+    <t>No comments in the code</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/nvariants.py", line 52, in &lt;module&gt;
+    nvariants()
+  File "/home/math/siglersa/raresim/nvariants.py", line 38, in nvariants
+    args = get_args()
+  File "/home/math/siglersa/raresim/nvariants.py", line 32, in get_args
+    if (not args.phi or not args.omega) and not args.pop:
+AttributeError: 'Namespace' object has no attribute 'omega'
+In the nvariants.py script, line 20 has dest = 'alpha', but I think it should be dest='omega'</t>
+    </r>
+  </si>
+  <si>
+    <t>Examples could be more descriptive</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1939,6 +1987,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2543,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2858,7 +2907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -3335,7 +3384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881D6BD8-94B7-4767-8C3D-2BA210E4CAAA}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3540,7 +3589,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>145</v>
       </c>
@@ -3566,17 +3615,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B57A4DD-947A-4B6A-8176-CE02EE70EDC3}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="119" customWidth="1"/>
     <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="3" max="3" width="61" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="22.21875" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" customWidth="1"/>
@@ -3597,9 +3646,8 @@
       <c r="A3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -3654,7 +3702,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3678,12 +3726,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3691,7 +3742,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3701,7 +3755,9 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -3752,6 +3808,17 @@
       </c>
       <c r="C23" s="9" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="18" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3764,6 +3831,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3771,8 +3839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75856291-DF21-4AFA-91C0-857E3D86DCEF}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3886,7 +3954,7 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3902,7 +3970,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="9"/>
     </row>
@@ -3960,12 +4028,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4192,28 +4270,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4238,12 +4309,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added note about added -sample to output name for extract.py
</commit_message>
<xml_diff>
--- a/Results/raresim_Beta Testing_Tracker.xlsx
+++ b/Results/raresim_Beta Testing_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15F4D07-1E77-42EE-A22A-7614892E78AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B35A9FE-67F9-41B2-A22A-1C9E405721F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-13044" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="156">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1854,6 +1854,12 @@
   </si>
   <si>
     <t>Examples could be more descriptive</t>
+  </si>
+  <si>
+    <t>Need work</t>
+  </si>
+  <si>
+    <t>I wouldn't add the -sample to the name of the output file. User should be able to name the output file exactly as specified in the -o line.</t>
   </si>
 </sst>
 </file>
@@ -2592,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2774,10 +2780,13 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>154</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>53</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3839,7 +3848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75856291-DF21-4AFA-91C0-857E3D86DCEF}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4028,25 +4037,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C8DD2C9503A9346957BF8010701C0C0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b8ca09d58466ecec5e066a1529d2c3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44ad9495-3741-4708-b440-876241155999" xmlns:ns3="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1aaa8f036973ab99e5e154ba7cda0df4" ns2:_="" ns3:_="">
     <xsd:import namespace="44ad9495-3741-4708-b440-876241155999"/>
@@ -4269,6 +4259,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4279,17 +4288,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F9A326-63A4-415F-BAD0-FF0443491DD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4308,6 +4306,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>

</xml_diff>